<commit_message>
Added Function key requirements
</commit_message>
<xml_diff>
--- a/SuperChatRequirements.xlsx
+++ b/SuperChatRequirements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>R001</t>
   </si>
@@ -101,9 +101,6 @@
     <t>R013</t>
   </si>
   <si>
-    <t>If a "Chat Room" is not selected by any user for more than 15 minutes its name shall be blanked out</t>
-  </si>
-  <si>
     <t>R014</t>
   </si>
   <si>
@@ -192,6 +189,21 @@
   </si>
   <si>
     <t>Users shall be able to see the list of all users by clicking &lt;F2&gt;</t>
+  </si>
+  <si>
+    <t>If a "Chat Room" is not selected by any user for more than 5 minutes its name shall be blanked out</t>
+  </si>
+  <si>
+    <t>R029</t>
+  </si>
+  <si>
+    <t>Users shall be able to change their Nick by clicking &lt;F3&gt;</t>
+  </si>
+  <si>
+    <t>R030</t>
+  </si>
+  <si>
+    <t>Users shall be able to exit SuperChat by clicking &lt;F4&gt;</t>
   </si>
 </sst>
 </file>
@@ -509,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,130 +633,147 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
         <v>41</v>
-      </c>
-      <c r="B22" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
         <v>52</v>
-      </c>
-      <c r="B27" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
         <v>54</v>
       </c>
-      <c r="B28" t="s">
-        <v>55</v>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>